<commit_message>
Excel: botón HEFAME con plantilla Transfer Hefame; Excel estándar sin plantilla
- Excel principal: siempre generado desde cero (imprimir cualquier pedido)
- Nuevo GET /pedidos/:id/hefame.xlsx con plantilla y mapeo: F5, C13-C16, líneas B21+ (Cantidad, CN, Descripción, Descuento)
- Botón HEFAME en vista pedido
- Plantilla PLANTILLA TRANSFER DIRECTO CRM.xlsx actualizada; README con mapeo

Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/templates/PLANTILLA TRANSFER DIRECTO CRM.xlsx
+++ b/templates/PLANTILLA TRANSFER DIRECTO CRM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pacol\iCloudDrive\01 FARMADESCANSO SL\02 PEDIDOS\01 GEMAVIP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pacol\CURSOR\CRM_Gemavip\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C0BE642-60B8-4E9B-8E17-194D7691D1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB27970E-8784-4246-8D93-B72BA8F86CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{43D4710E-17FA-46CC-9775-DF7A3B84A70C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>COMUNICACIÓN DE TRANSFER</t>
   </si>
@@ -86,27 +86,6 @@
     <t>Cantidad Bonificada</t>
   </si>
   <si>
-    <t>IALOZON BLU COLUTORIO</t>
-  </si>
-  <si>
-    <t>IALOZON BLU PASTA</t>
-  </si>
-  <si>
-    <t>IALOZON ROSA COLUTORIO</t>
-  </si>
-  <si>
-    <t>IALOZON ROSA PASTA</t>
-  </si>
-  <si>
-    <t>IALOZON SUPERHIDRATANTE COLUTORIO</t>
-  </si>
-  <si>
-    <t>IALOZON GEL ORAL</t>
-  </si>
-  <si>
-    <t>IALOZON CLEAN</t>
-  </si>
-  <si>
     <t>* cada pedido transfer debe llevar dto o bonificiacion ( no ambas opciones en el mismo transfer)</t>
   </si>
   <si>
@@ -120,15 +99,6 @@
   </si>
   <si>
     <t>TRANSFER COMPARTIDO</t>
-  </si>
-  <si>
-    <t>30550 Abarán Murcia ES</t>
-  </si>
-  <si>
-    <t>GÓMEZ ABELLÁN, JESÚS JOAQUÍN</t>
-  </si>
-  <si>
-    <t>968770478</t>
   </si>
 </sst>
 </file>
@@ -504,15 +474,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>933450</xdr:colOff>
+      <xdr:colOff>898945</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>135147</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:colOff>70270</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>30372</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -542,8 +512,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5835650" y="152400"/>
-          <a:ext cx="1743075" cy="441325"/>
+          <a:off x="6894303" y="135147"/>
+          <a:ext cx="1707492" cy="455942"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -898,7 +868,7 @@
   <dimension ref="B3:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="12.9" x14ac:dyDescent="0.2"/>
@@ -1381,10 +1351,10 @@
     </row>
     <row r="7" spans="2:6" ht="27.85" x14ac:dyDescent="0.3">
       <c r="B7" s="28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -1392,7 +1362,7 @@
     </row>
     <row r="8" spans="2:6" ht="27.85" x14ac:dyDescent="0.3">
       <c r="B8" s="28" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="7"/>
@@ -1401,7 +1371,7 @@
     </row>
     <row r="9" spans="2:6" ht="27.85" x14ac:dyDescent="0.3">
       <c r="B9" s="28" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="7"/>
@@ -1435,9 +1405,7 @@
       <c r="B13" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>29</v>
-      </c>
+      <c r="C13" s="13"/>
       <c r="D13" s="30"/>
       <c r="E13" s="14"/>
       <c r="F13" s="15"/>
@@ -1446,9 +1414,7 @@
       <c r="B14" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="13">
-        <v>17308</v>
-      </c>
+      <c r="C14" s="13"/>
       <c r="D14" s="30"/>
       <c r="E14" s="14"/>
       <c r="F14" s="15"/>
@@ -1457,9 +1423,7 @@
       <c r="B15" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="C15" s="13"/>
       <c r="D15" s="30"/>
       <c r="E15" s="14"/>
       <c r="F15" s="15"/>
@@ -1468,9 +1432,7 @@
       <c r="B16" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="18" t="s">
-        <v>28</v>
-      </c>
+      <c r="C16" s="18"/>
       <c r="D16" s="31"/>
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
@@ -1518,113 +1480,57 @@
       </c>
     </row>
     <row r="21" spans="2:6" ht="15.65" x14ac:dyDescent="0.25">
-      <c r="B21" s="25">
-        <v>0</v>
-      </c>
-      <c r="C21" s="25">
-        <v>135990</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="27">
-        <v>0</v>
-      </c>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="27"/>
       <c r="F21" s="25"/>
     </row>
     <row r="22" spans="2:6" ht="15.65" x14ac:dyDescent="0.25">
-      <c r="B22" s="25">
-        <v>0</v>
-      </c>
-      <c r="C22" s="25">
-        <v>135988</v>
-      </c>
-      <c r="D22" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="27">
-        <v>0</v>
-      </c>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="27"/>
       <c r="F22" s="25"/>
     </row>
     <row r="23" spans="2:6" ht="15.65" x14ac:dyDescent="0.25">
-      <c r="B23" s="25">
-        <v>0</v>
-      </c>
-      <c r="C23" s="25">
-        <v>135991</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="27">
-        <v>0</v>
-      </c>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="27"/>
       <c r="F23" s="25"/>
     </row>
     <row r="24" spans="2:6" ht="15.65" x14ac:dyDescent="0.25">
-      <c r="B24" s="25">
-        <v>0</v>
-      </c>
-      <c r="C24" s="25">
-        <v>135989</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24" s="27">
-        <v>0</v>
-      </c>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="27"/>
       <c r="F24" s="25"/>
     </row>
     <row r="25" spans="2:6" ht="15.65" x14ac:dyDescent="0.25">
-      <c r="B25" s="25">
-        <v>0</v>
-      </c>
-      <c r="C25" s="25">
-        <v>135993</v>
-      </c>
-      <c r="D25" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="27">
-        <v>0</v>
-      </c>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="27"/>
       <c r="F25" s="25"/>
     </row>
     <row r="26" spans="2:6" ht="15.65" x14ac:dyDescent="0.25">
-      <c r="B26" s="25">
-        <v>0</v>
-      </c>
-      <c r="C26" s="25">
-        <v>135992</v>
-      </c>
-      <c r="D26" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="27">
-        <v>0.05</v>
-      </c>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="27"/>
       <c r="F26" s="25"/>
     </row>
     <row r="27" spans="2:6" ht="15.65" x14ac:dyDescent="0.25">
-      <c r="B27" s="25">
-        <v>0</v>
-      </c>
-      <c r="C27" s="25">
-        <v>135994</v>
-      </c>
-      <c r="D27" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" s="27">
-        <v>0</v>
-      </c>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="27"/>
       <c r="F27" s="25"/>
     </row>
     <row r="28" spans="2:6" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B28" s="34" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>

</xml_diff>